<commit_message>
Adding remaining In/out and week 2
1. Adding Input/Output remaining methods (POI and Properties)
2. Singleton
3. Enum
</commit_message>
<xml_diff>
--- a/src/InOut/Resources/Excel.xlsx
+++ b/src/InOut/Resources/Excel.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Datatype</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>No fixed size</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
 </sst>
 </file>
@@ -149,8 +146,8 @@
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
-        <v>11</v>
+      <c r="C5" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="6">

</xml_diff>